<commit_message>
update sprint project dan team detail
</commit_message>
<xml_diff>
--- a/team_details.xlsx
+++ b/team_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DOKUMEN\Kuliah\Semester7\Prak. Pembelajaran Mesin\PraktikumML_073-076\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E169672-0B85-4BEC-8FCA-CE821A176516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0283973D-0554-444B-A5C2-3EF15B186746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Anggota Kelompok</t>
   </si>
@@ -55,16 +55,45 @@
   </si>
   <si>
     <t>Sumber Artikel</t>
+  </si>
+  <si>
+    <t>Convolutional neural network for maize leaf disease image classification</t>
+  </si>
+  <si>
+    <t>https://github.com/spMohanty/PlantVillage-Dataset</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.12928/telkomnika.v18i3.14840</t>
+  </si>
+  <si>
+    <t>PlantVillage</t>
+  </si>
+  <si>
+    <t>Prosedur komputasi untuk pengenalan dan klasifikasi penyakit daun jagung dari daun sehat menggunakan metode CNN</t>
+  </si>
+  <si>
+    <t>NIM : 201810370311073</t>
+  </si>
+  <si>
+    <t>NIM : 201810370311076</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -196,10 +225,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -210,8 +240,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,7 +525,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +534,7 @@
     <col min="2" max="2" width="6.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -516,7 +548,9 @@
         <v>2</v>
       </c>
       <c r="D1" s="8"/>
-      <c r="E1" s="9"/>
+      <c r="E1" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
@@ -527,14 +561,18 @@
         <v>3</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
     </row>
@@ -545,7 +583,9 @@
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
     </row>
@@ -554,7 +594,9 @@
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
     </row>
@@ -565,7 +607,9 @@
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
     </row>
@@ -574,11 +618,17 @@
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{5F02F33E-B004-4A87-A976-96CAB35148A2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>